<commit_message>
Complete with ref lists
</commit_message>
<xml_diff>
--- a/PS00.xlsx
+++ b/PS00.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lloydsregistergroup.sharepoint.com/sites/group-proj-energyprj11100223773/Shared Documents/6. Project Work place/21 PS/treeline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drsun\OneDrive\Desktop\RUBY_PS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{EB3C04AD-BFBD-4486-8496-142081C6361A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{5CEA9906-8683-4267-9BC4-9CBA3B9E439E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8D7EB-59B4-4CA5-986D-A9A88E90E6FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="3675" windowWidth="12150" windowHeight="20835" xr2:uid="{D8F3E331-1E84-40A9-9AED-BF4A3C948703}"/>
+    <workbookView xWindow="11930" yWindow="3010" windowWidth="25950" windowHeight="16530" activeTab="2" xr2:uid="{D8F3E331-1E84-40A9-9AED-BF4A3C948703}"/>
   </bookViews>
   <sheets>
     <sheet name="00" sheetId="1" r:id="rId1"/>
+    <sheet name="RulesReg" sheetId="2" r:id="rId2"/>
+    <sheet name="InputDocs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,23 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
-  <si>
-    <t>PS-16 Temporary refuge (TR)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Goal/objective</t>
   </si>
   <si>
-    <t>Element Goal</t>
-  </si>
-  <si>
-    <t>System boundary</t>
-  </si>
-  <si>
-    <t>Subelement Name</t>
-  </si>
-  <si>
     <t>FUNCTIONALITY</t>
   </si>
   <si>
@@ -78,12 +68,6 @@
     <t>Event</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>Corresponding MAH(S)</t>
-  </si>
-  <si>
     <t>Dependencies/interactions</t>
   </si>
   <si>
@@ -93,14 +77,41 @@
     <t>Interaction/dependency</t>
   </si>
   <si>
-    <t>PS Ref.</t>
+    <t>PS-## SCE</t>
+  </si>
+  <si>
+    <t>Sub-element</t>
+  </si>
+  <si>
+    <t>Rules &amp; Regulations</t>
+  </si>
+  <si>
+    <t>Doc No</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>Input Documents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,19 +141,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Frutiger LT 45 Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Frutiger LT 45 Light"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF111111"/>
       <name val="Frutiger LT 45 Light"/>
       <family val="2"/>
     </font>
@@ -169,12 +168,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE5E5E5"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
@@ -188,6 +181,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="65"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,8 +264,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -274,69 +286,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,295 +627,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BA4275-9CBB-4EB1-BFB5-2D65780E7CE0}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="11.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="B9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="9"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:E24"/>
+  <mergeCells count="12">
+    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="B18:F18"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876CB04A-5648-4582-8C8A-5E2FD91F5796}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="45.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730DF998-6B4D-4CAB-A829-AE982D1516EE}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="26.7265625" customWidth="1"/>
+    <col min="5" max="5" width="45.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>